<commit_message>
refactor: modify the file excel
</commit_message>
<xml_diff>
--- a/assets/plantas.xlsx
+++ b/assets/plantas.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Dolencia,Planta</t>
   </si>
   <si>
-    <t xml:space="preserve">tos,eucalipto,El eucalipto es una planta que ayuda a respirar  mejor cuando tienes tos. Tiene un aceite que saca la mucosidad de los pulmones, mata los gérmenes que te enferman, calma el dolor de la garganta y baja la inflamación. Puedes usar el eucalipto de tres maneras: Tomar un té de eucalipto: pon una cucharada de hojas de eucalipto en una taza de agua hirviendo. Déjalo reposar 10 minutos y cuélalo. Añade miel si quieres. Toma dos o tres tazas al día. Respirar el vapor de eucalipto: pon unas gotas de aceite de eucalipto en un recipiente con agua caliente. Cubre tu cabeza con una toalla y respira el vapor que sale. Hazlo 10 o 15 minutos, dos o tres veces al día. Ten cuidado de no quemarte. Poner un ungüento de eucalipto: compra o haz un ungüento o bálsamo de eucalipto. Ponlo en el pecho y la espalda y masajea suavemente. Esto te ayuda a despejar las vías respiratorias y a relajar los músculos. Hazlo dos o tres veces al día. El eucalipto es natural y seguro, pero consulta con tu médico antes de usarlo si eres alérgico, tienes alguna enfermedad o estás embarazada.</t>
+    <t xml:space="preserve">tos,eucalipto-El eucalipto es una planta que ayuda a respirar  mejor cuando tienes tos. Tiene un aceite que saca la mucosidad de los pulmones, mata los gérmenes que te enferman, calma el dolor de la garganta y baja la inflamación. Puedes usar el eucalipto de tres maneras: Tomar un té de eucalipto: pon una cucharada de hojas de eucalipto en una taza de agua hirviendo. Déjalo reposar 10 minutos y cuélalo. Añade miel si quieres. Toma dos o tres tazas al día. Respirar el vapor de eucalipto: pon unas gotas de aceite de eucalipto en un recipiente con agua caliente. Cubre tu cabeza con una toalla y respira el vapor que sale. Hazlo 10 o 15 minutos, dos o tres veces al día. Ten cuidado de no quemarte. Poner un ungüento de eucalipto: compra o haz un ungüento o bálsamo de eucalipto. Ponlo en el pecho y la espalda y masajea suavemente. Esto te ayuda a despejar las vías respiratorias y a relajar los músculos. Hazlo dos o tres veces al día. El eucalipto es natural y seguro, pero consulta con tu médico antes de usarlo si eres alérgico, tienes alguna enfermedad o estás embarazada.</t>
   </si>
   <si>
     <t xml:space="preserve">gripe,jengibre-El jengibre es una raíz que tiene propiedades antivirales, antiinflamatorias, expectorantes y analgésicas. Ayuda a combatir la gripe al fortalecer el sistema inmunológico, aliviar los síntomas como la fiebre, el dolor de cabeza, la congestión nasal y la tos, y acelerar la recuperación. Puedes usar el jengibre de varias maneras: Tomar un té de jengibre: ralla un trozo de jengibre fresco y ponlo en una taza de agua hirviendo. Déjalo reposar 10 minutos y cuélalo. Añade limón y miel si quieres. Toma tres o cuatro tazas al día. Masticar un trozo de jengibre: pela y corta un trozo de jengibre fresco y mastícalo lentamente. Esto te ayudará a despejar la garganta y la nariz. Hazlo dos o tres veces al día. Hacer un jarabe de jengibre: mezcla media taza de jugo de jengibre, media taza de jugo de limón y media taza de miel en un frasco. Agita bien y toma una cucharada cada dos horas. Guarda el jarabe en el refrigerador. El jengibre es natural y seguro, pero consulta con tu médico antes de usarlo si tienes problemas de coagulación, presión arterial alta o diabetes.</t>
@@ -264,7 +264,7 @@
   <dimension ref="A1:A1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
refactor: mofify plants excel
</commit_message>
<xml_diff>
--- a/assets/plantas.xlsx
+++ b/assets/plantas.xlsx
@@ -25,39 +25,10 @@
     <t xml:space="preserve">Dolencia,Planta</t>
   </si>
   <si>
-    <t xml:space="preserve">tos,eucalipto-El eucalipto es una planta que tiene propiedades antiinflamatorias, antibacterianas y expectorantes. Esto significa que puede ayudar a aliviar la inflamación de las vías respiratorias, matar las bacterias que causan la infección y ayudar a expulsar la mucosidad.
-Hay tres formas principales de usar el eucalipto para la tos:
-1. Tomar té de eucalipto
-Para hacer té de eucalipto, sigue estos pasos:
-Pon una cucharada de hojas de eucalipto en una taza de agua hirviendo.
-Déjalo reposar 10 minutos.
-Cuélalo.
-Añade miel si quieres.
-Puedes tomar dos o tres tazas de té de eucalipto al día.
-2. Respirar vapor de eucalipto
-Para respirar vapor de eucalipto, sigue estos pasos:
-Pon unas gotas de aceite de eucalipto en un recipiente con agua caliente.
-Cubre tu cabeza con una toalla y respira el vapor que sale.
-Hazlo 10 o 15 minutos, dos o tres veces al día.
-Ten cuidado de no quemarte.
-3. Poner un ungüento de eucalipto
-Para poner un ungüento de eucalipto, sigue estos pasos:
-Compra o haz un ungüento o bálsamo de eucalipto.
-Ponlo en el pecho y la espalda y masajea suavemente.
-Hazlo dos o tres veces al día.
-Esto te ayuda a despejar las vías respiratorias y a relajar los músculos.
-Precauciones
-El eucalipto es natural y seguro, pero consulta con tu médico antes de usarlo si eres alérgico, tienes alguna enfermedad o estás embarazada.
-Otros consejos
-Además de usar eucalipto, hay otros consejos que pueden ayudarte a aliviar la tos:
-Bebe mucho líquido.
-Haz gárgaras con agua salada.
-Humedece el aire de tu habitación con un humidificador.
-Duerme con la cabeza elevada.
-Si la tos es persistente o grave, consulta con tu médico.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gripe,jengibre-El jengibre es una raíz que tiene propiedades antivirales, antiinflamatorias, expectorantes y analgésicas. Ayuda a combatir la gripe al fortalecer el sistema inmunológico, aliviar los síntomas como la fiebre, el dolor de cabeza, la congestión nasal y la tos, y acelerar la recuperación. Puedes usar el jengibre de varias maneras: Tomar un té de jengibre: ralla un trozo de jengibre fresco y ponlo en una taza de agua hirviendo. Déjalo reposar 10 minutos y cuélalo. Añade limón y miel si quieres. Toma tres o cuatro tazas al día. Masticar un trozo de jengibre: pela y corta un trozo de jengibre fresco y mastícalo lentamente. Esto te ayudará a despejar la garganta y la nariz. Hazlo dos o tres veces al día. Hacer un jarabe de jengibre: mezcla media taza de jugo de jengibre, media taza de jugo de limón y media taza de miel en un frasco. Agita bien y toma una cucharada cada dos horas. Guarda el jarabe en el refrigerador. El jengibre es natural y seguro, pero consulta con tu médico antes de usarlo si tienes problemas de coagulación, presión arterial alta o diabetes.</t>
+    <t xml:space="preserve">tos,eucalipto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gripe,jengibre</t>
   </si>
   <si>
     <t xml:space="preserve">quemaduras,siempreviva-La siempreviva es una planta que tiene propiedades cicatrizantes, regeneradoras, antisépticas y antiinflamatorias. Ayuda a curar las quemaduras al proteger la piel, evitar las infecciones, reducir el dolor y el enrojecimiento, y favorecer la formación de tejido nuevo. Puedes usar la siempreviva de dos maneras: Aplicar el gel de siempreviva: corta una hoja de siempreviva y extrae el gel que contiene. Lava la quemadura con agua fría y sécala con una gasa estéril. Aplica el gel sobre la quemadura y cubre con una gasa. Cambia el vendaje dos veces al día. Tomar un jugo de siempreviva: licua una hoja de siempreviva con un vaso de agua. Cuela y bebe el jugo en ayunas. Esto te ayudará a desintoxicar el organismo y a mejorar la cicatrización. Hazlo una vez al día. La siempreviva es natural y segura, pero consulta con tu médico antes de usarla si eres alérgico, tienes alguna enfermedad o estás embarazada.</t>
@@ -260,7 +231,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -271,10 +242,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -297,7 +264,7 @@
   <dimension ref="A1:A1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -310,8 +277,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="572.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: add plants excels
</commit_message>
<xml_diff>
--- a/assets/plantas.xlsx
+++ b/assets/plantas.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="44">
   <si>
     <t xml:space="preserve">Dolencia,Planta</t>
   </si>
@@ -31,34 +31,106 @@
     <t xml:space="preserve">gripe,jengibre</t>
   </si>
   <si>
-    <t xml:space="preserve">quemaduras,siempreviva-La siempreviva es una planta que tiene propiedades cicatrizantes, regeneradoras, antisépticas y antiinflamatorias. Ayuda a curar las quemaduras al proteger la piel, evitar las infecciones, reducir el dolor y el enrojecimiento, y favorecer la formación de tejido nuevo. Puedes usar la siempreviva de dos maneras: Aplicar el gel de siempreviva: corta una hoja de siempreviva y extrae el gel que contiene. Lava la quemadura con agua fría y sécala con una gasa estéril. Aplica el gel sobre la quemadura y cubre con una gasa. Cambia el vendaje dos veces al día. Tomar un jugo de siempreviva: licua una hoja de siempreviva con un vaso de agua. Cuela y bebe el jugo en ayunas. Esto te ayudará a desintoxicar el organismo y a mejorar la cicatrización. Hazlo una vez al día. La siempreviva es natural y segura, pero consulta con tu médico antes de usarla si eres alérgico, tienes alguna enfermedad o estás embarazada.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">acne,malva-La malva es una planta que tiene propiedades emolientes, antiinflamatorias, astringentes y antibacterianas. Ayuda a tratar el acné al limpiar la piel, eliminar el exceso de grasa, desinflamar los poros, prevenir las infecciones y suavizar la piel. Puedes usar la malva de dos maneras: Hacer una mascarilla de malva: pon un puñado de hojas y flores de malva en una olla con agua y déjalas hervir 10 minutos. Cuela y deja enfriar. Tritura las hojas y flores con un tenedor y forma una pasta. Aplica la pasta sobre el rostro limpio y deja actuar 20 minutos. Enjuaga con agua tibia y seca con una toalla suave. Hazlo dos o tres veces por semana. Hacer un tónico de malva: pon un puñado de hojas y flores de malva en una olla con agua y déjalas hervir 10 minutos. Cuela y deja enfriar. Guarda el líquido en una botella. Aplica el tónico sobre el rostro con un algodón después de lavarte la cara. Hazlo dos veces al día. La malva es natural y segura, pero consulta con tu médico antes de usarla si eres alérgico, tienes alguna enfermedad o estás embarazada.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">náuseas,jengibre-El jengibre es una raíz que tiene propiedades antieméticas, digestivas, carminativas y antiespasmódicas. Ayuda a aliviar las náuseas al calmar el estómago, estimular la producción de saliva y bilis, expulsar los gases y relajar los músculos intestinales. Puedes usar el jengibre de varias maneras: Tomar un té de jengibre: ralla un trozo de jengibre fresco y ponlo en una taza de agua hirviendo. Déjalo reposar 10 minutos y cuélalo. Añade limón y miel si quieres. Toma una taza cuando sientas náuseas. Comer un caramelo de jengibre: compra o haz caramelos de jengibre. Chupa un caramelo cuando sientas náuseas. Esto te ayudará a estimular la saliva y a calmar el estómago. Tomar una cápsula de jengibre: compra cápsulas de jengibre en una farmacia o tienda naturista. Toma una cápsula con un vaso de agua cuando sientas náuseas. Sigue las instrucciones del envase. El jengibre es natural y seguro, pero consulta con tu médico antes de usarlo si tienes problemas de coagulación, presión arterial alta o diabetes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">alergia,alparraco-El alparraco es una planta que tiene propiedades antihistamínicas, antiinflamatorias, antialérgicas y expectorantes. Ayuda a combatir la alergia al bloquear la liberación de histamina, aliviar los síntomas como la congestión nasal, el picor de ojos, la tos y el estornudo, y eliminar las secreciones. Puedes usar el alparraco de dos maneras: Tomar un té de alparraco: pon una cucharada de hojas de alparraco en una taza de agua hirviendo. Déjalo reposar 10 minutos y cuélalo. Añade miel si quieres. Toma dos o tres tazas al día. Hacer un lavado nasal con alparraco: pon una cucharada de hojas de alparraco en una olla con agua y déjalas hervir 10 minutos. Cuela y deja enfriar. Llena una jeringa o un irrigador nasal con el líquido. Introduce la punta en una fosa nasal y aprieta suavemente. Repite con la otra fosa nasal. Hazlo dos veces al día. El alparraco es natural y seguro, pero consulta con tu médico antes de usarlo si eres alérgico, tienes alguna enfermedad o estás embarazado.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">insomnio,manzanilla-La manzanilla es una planta que tiene propiedades sedantes, relajantes, antiespasmódicas y antidepresivas. Ayuda a combatir el insomnio al calmar los nervios, reducir la ansiedad, mejorar el ánimo, favorecer el sueño y relajar los músculos. Puedes usar la manzanilla de dos maneras: Tomar un té de manzanilla: pon una cucharadita de flores de manzanilla en una taza de agua hirviendo. Déjalo reposar 10 minutos y cuélalo. Añade miel si quieres. Toma una taza media hora antes de acostarte. Hacer una aromaterapia de manzanilla: pon unas gotas de aceite esencial de manzanilla en un difusor o un quemador de esencias. Enciende una vela y deja que el aroma se esparza por el ambiente. Respira profundamente y relájate. Hazlo una vez al día.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bronquitis,eucalipto-El eucalipto es una planta que ayuda a respirar mejor cuando tienes bronquitis. Tiene un aceite que saca la mucosidad de los bronquios, mata los gérmenes que te enferman, calma el dolor de la garganta y baja la inflamación. Puedes usar el eucalipto de tres maneras: Tomar un té de eucalipto: pon una cucharada de hojas de eucalipto en una taza de agua hirviendo. Déjalo reposar 10 minutos y cuélalo. Añade miel si quieres. Toma dos o tres tazas al día. Respirar el vapor de eucalipto: pon unas gotas de aceite de eucalipto en un recipiente con agua caliente. Cubre tu cabeza con una toalla y respira el vapor que sale. Hazlo 10 o 15 minutos, dos o tres veces al día. Ten cuidado de no quemarte. Poner un ungüento de eucalipto: compra o haz un ungüento o bálsamo de eucalipto. Ponlo en el pecho y la espalda y masajea suavemente. Esto te ayuda a despejar las vías respiratorias y a relajar los músculos. Hazlo dos o tres veces al día. El eucalipto es natural y seguro, pero consulta con tu médico antes de usarlo si eres alérgico, si tienes alguna enfermedad o estás embarazada.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">heridas,siempreviva- La siempreviva es una planta que tiene propiedades cicatrizantes, regeneradoras, antisépticas y antiinflamatorias. Ayuda a curar las heridas al proteger la piel, evitar las infecciones, reducir el dolor y el enrojecimiento, y favorecer la formación de tejido nuevo. Puedes usar la siempreviva de dos maneras: Aplicar el gel de siempreviva: corta una hoja de siempreviva y extrae el gel que contiene. Lava la herida con agua y jabón y sécala con una gasa estéril. Aplica el gel sobre la herida y cubre con una gasa. Cambia el vendaje dos veces al día. Tomar un jugo de siempreviva: licua una hoja de siempreviva con un vaso de agua. Cuela y bebe el jugo en ayunas. Esto te ayudará a desintoxicar el organismo y a mejorar la cicatrización. Hazlo una vez al día.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eccema,malva-La malva es una planta que tiene propiedades emolientes, antiinflamatorias, astringentes y antibacterianas. Ayuda a tratar el eccema al limpiar la piel, eliminar el exceso de grasa, desinflamar los poros, prevenir las infecciones y suavizar la piel. Puedes usar la malva de dos maneras: Hacer una compresa de malva: pon un puñado de hojas y flores de malva en una olla con agua y déjalas hervir 10 minutos. Cuela y deja enfriar. Empapa un paño limpio con el líquido y aplícalo sobre la zona afectada. Déjalo actuar 15 minutos y retira. Hazlo dos o tres veces al día. Hacer una crema de malva: mezcla una cucharada de gel de aloe vera con una cucharada de aceite de coco y una cucharada de infusión de malva. Guarda la crema en un frasco. Aplica la crema sobre la zona afectada y masajea suavemente. Hazlo dos o tres veces al día. La malva es natural y segura, pero consulta con tu médico antes de usarla si eres alérgico, tienes alguna enfermedad o estás embarazada.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">indigestión,jengibre-El jengibre es una raíz que tiene propiedades digestivas, carminativas, antiespasmódicas y antiinflamatorias. Ayuda a aliviar la indigestión al estimular la producción de saliva y bilis, expulsar los gases, relajar los músculos intestinales y prevenir las náuseas. Puedes usar el jengibre de varias maneras: Tomar un té de jengibre: ralla un trozo de jengibre fresco y ponlo en una taza de agua hirviendo. Déjalo reposar 10 minutos y cuélalo. Añade limón y miel si quieres. Toma una taza después de comer. Comer un trozo de jengibre: pela y corta un trozo de jengibre fresco y mastícalo lentamente. Esto te ayudará a estimular la digestión y a calmar el estómago. Hazlo después de comer. El jengibre es natural y seguro, pero consulta con tu médico antes de usarlo si tienes problemas de coagulación, presión arterial alta o diabetes.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">diarrea,alcaparro-El alcaparro enano es una planta que ayuda a tratar la diarrea al limpiar el intestino, eliminar las toxinas, prevenir las infecciones, reducir la inflamación y favorecer la cicatrización de las mucosas. Puedes usar el alcaparro enano de dos maneras: Tomar un té de alcaparro enano: pon una cucharadita de hojas y flores de alcaparro enano en una taza de agua hirviendo. Déjalo reposar 10 minutos y cuélalo. Añade miel si quieres. Toma una taza en ayunas y otra antes de acostarte. Esto te ayudará a regular el tránsito intestinal y a aliviar el malestar.</t>
+    <t xml:space="preserve">indigestion,menta_silvestre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acidez,manzanilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">artritis,alparraco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quemaduras,siempreviva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ansiedad,manzanilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fatiga,jengibre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asma,eucalipto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">desintoxicado,alparraco</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">estreñimiento,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">alparraco</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">ulcera,siempreviva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conjuntivitis,manzanilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hemorroides,alparraco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nauseas,jengibre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bronquitis,eucalipto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">colico,menta_silvestre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catarro,manzanilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">herida,siempreviva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vomito,jengibre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">menstruacion,manzanilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">picaduras,malva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mareos,jengibre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">acne,malva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">alergia,alparraco</t>
+  </si>
+  <si>
+    <t xml:space="preserve">insomnio,manzanilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heridas,siempreviva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eccema,malva</t>
+  </si>
+  <si>
+    <t xml:space="preserve">indigestión,jengibre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diarrea,alcaparro</t>
   </si>
   <si>
     <t xml:space="preserve">depresión,manzanilla</t>
@@ -79,9 +151,6 @@
     <t xml:space="preserve">dermatitis,malva</t>
   </si>
   <si>
-    <t xml:space="preserve">mareos,jengibre</t>
-  </si>
-  <si>
     <t xml:space="preserve">rinitis,alparraco</t>
   </si>
   <si>
@@ -100,55 +169,7 @@
     <t xml:space="preserve">hemorroides,siempreviva</t>
   </si>
   <si>
-    <t xml:space="preserve">acidez,malva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conjuntivitis,alparraco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gingivitis,menta silvestre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cistitis,eucalipto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ansiedad,valeriana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">verrugas,siempreviva</t>
-  </si>
-  <si>
     <t xml:space="preserve">diarrea,malva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">otitis,alparraco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gastritis,manzanilla</t>
-  </si>
-  <si>
-    <t xml:space="preserve">faringitis,eucalipto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">insomnio,valeriana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">quemadurassolares,siempreviva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">estreñimiento,malva</t>
-  </si>
-  <si>
-    <t xml:space="preserve">resaca,jengibre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">urticaria,alparraco</t>
-  </si>
-  <si>
-    <t xml:space="preserve">aftas,menta silvestre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">amigdalitis,eucalipto</t>
   </si>
 </sst>
 </file>
@@ -158,7 +179,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -187,6 +208,12 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
   </fonts>
   <fills count="2">
@@ -263,8 +290,8 @@
   </sheetPr>
   <dimension ref="A1:A1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A27" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A47" activeCellId="0" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -327,7 +354,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
@@ -399,62 +426,62 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -469,27 +496,27 @@
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -502,6 +529,57 @@
         <v>42</v>
       </c>
     </row>
+    <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2"/>
+    </row>
+    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2"/>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2"/>
+    </row>
+    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2"/>
+    </row>
+    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2"/>
+    </row>
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="2"/>
+    </row>
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="2"/>
+    </row>
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="2"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="2"/>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="2"/>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="2"/>
+    </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>